<commit_message>
fix(content): correct Spanish text encoding and improve generators
- Add proper Spanish accents (á, é, í, ó, ú, ñ) across all module
  documentation and reference files
- Fix Markdown table generation to handle newlines in cells
- Correct Excel named table styling to avoid conflicts with manual formatting
- Prefix formula-like text with space to prevent Excel interpretation errors
- Update cancelled invoice handling in data cleaning exercise (gen_04)
- Regenerate all Excel output files with corrected content
</commit_message>
<xml_diff>
--- a/output/Pack_Excel_Pro/Modulo_1_Funciones/01_Calculadora_ISR_V2026.xlsx
+++ b/output/Pack_Excel_Pro/Modulo_1_Funciones/01_Calculadora_ISR_V2026.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarifa_Anual_2026" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarifa_Mensual_2026" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Calculadora_ISR" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Actualizacion_CFF" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ejercicios" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrucciones" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Tarifa_Anual_2026" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tarifa_Mensual_2026" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Calculadora_ISR" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Actualizacion_CFF" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Ejercicios" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Instrucciones" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -41,9 +41,8 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="11"/>
+      <color rgb="00475569"/>
+      <sz val="9"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -52,14 +51,15 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <color rgb="00475569"/>
-      <sz val="9"/>
+      <b val="1"/>
+      <color rgb="001E293B"/>
+      <sz val="12"/>
     </font>
     <font>
       <name val="Calibri"/>
       <b val="1"/>
-      <color rgb="001E293B"/>
-      <sz val="12"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="6">
@@ -71,22 +71,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00F59E0B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0010B981"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="002563EB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00F8FAFC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F59E0B"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0010B981"/>
       </patternFill>
     </fill>
   </fills>
@@ -121,24 +121,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="4" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -147,19 +134,28 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -583,180 +579,180 @@
     </row>
     <row r="2"/>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Límite Inferior</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Límite Superior</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Cuota Fija</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>% Sobre Excedente</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="2" t="n">
         <v>10135.11</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="3" t="n">
         <v>0.0192</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="2" t="n">
         <v>10135.12</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="2" t="n">
         <v>86022.11</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="2" t="n">
         <v>194.59</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="3" t="n">
         <v>0.064</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="2" t="n">
         <v>86022.12</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="2" t="n">
         <v>151176.19</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="2" t="n">
         <v>5051.37</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="3" t="n">
         <v>0.1088</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="2" t="n">
         <v>151176.2</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="2" t="n">
         <v>175735.66</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="2" t="n">
         <v>12140.13</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="3" t="n">
         <v>0.16</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="2" t="n">
         <v>175735.67</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="2" t="n">
         <v>210403.69</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="2" t="n">
         <v>16069.64</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="3" t="n">
         <v>0.1792</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="2" t="n">
         <v>210403.7</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="2" t="n">
         <v>424353.97</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="2" t="n">
         <v>22282.14</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="3" t="n">
         <v>0.2136</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="2" t="n">
         <v>424353.98</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="2" t="n">
         <v>668840.14</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="2" t="n">
         <v>67981.92</v>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="D10" s="3" t="n">
         <v>0.2352</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="2" t="n">
         <v>668840.15</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="2" t="n">
         <v>1276925.98</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="2" t="n">
         <v>125485.07</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="3" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="2" t="n">
         <v>1276925.99</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="2" t="n">
         <v>1702567.97</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="2" t="n">
         <v>307910.81</v>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D12" s="3" t="n">
         <v>0.32</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="2" t="n">
         <v>1702567.98</v>
       </c>
-      <c r="B13" s="5" t="n">
+      <c r="B13" s="2" t="n">
         <v>5107703.92</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="2" t="n">
         <v>444116.23</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="3" t="n">
         <v>0.34</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="2" t="n">
         <v>5107703.93</v>
       </c>
-      <c r="B14" s="3" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>En adelante</t>
         </is>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="2" t="n">
         <v>1601862.46</v>
       </c>
-      <c r="D14" s="4" t="n">
+      <c r="D14" s="3" t="n">
         <v>0.35</v>
       </c>
     </row>
@@ -802,178 +798,178 @@
     </row>
     <row r="2"/>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Límite Inferior</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Límite Superior</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Cuota Fija</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>% Sobre Excedente</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="2" t="n">
         <v>844.59</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="3" t="n">
         <v>0.0192</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="2" t="n">
         <v>844.6</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="2" t="n">
         <v>7168.51</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="2" t="n">
         <v>16.22</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="3" t="n">
         <v>0.064</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="2" t="n">
         <v>7168.52</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="2" t="n">
         <v>12598.02</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="2" t="n">
         <v>420.95</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="3" t="n">
         <v>0.1088</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="2" t="n">
         <v>12598.03</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="2" t="n">
         <v>14644.64</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="2" t="n">
         <v>1011.68</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="3" t="n">
         <v>0.16</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="2" t="n">
         <v>14644.65</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="2" t="n">
         <v>17533.64</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="2" t="n">
         <v>1339.14</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="3" t="n">
         <v>0.1792</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="2" t="n">
         <v>17533.65</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="2" t="n">
         <v>35362.83</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="2" t="n">
         <v>1856.84</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="3" t="n">
         <v>0.2136</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="2" t="n">
         <v>35362.84</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="2" t="n">
         <v>55736.68</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="2" t="n">
         <v>5665.16</v>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="D10" s="3" t="n">
         <v>0.2352</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="2" t="n">
         <v>55736.69</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="2" t="n">
         <v>106410.5</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="2" t="n">
         <v>10457.09</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="3" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="2" t="n">
         <v>106410.51</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="2" t="n">
         <v>141880.66</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="2" t="n">
         <v>25659.23</v>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D12" s="3" t="n">
         <v>0.32</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="2" t="n">
         <v>141880.67</v>
       </c>
-      <c r="B13" s="5" t="n">
+      <c r="B13" s="2" t="n">
         <v>425641.99</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="2" t="n">
         <v>37009.69</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="3" t="n">
         <v>0.34</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="2" t="n">
         <v>425642</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="2" t="n">
         <v>999999999</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="2" t="n">
         <v>133488.54</v>
       </c>
-      <c r="D14" s="4" t="n">
+      <c r="D14" s="3" t="n">
         <v>0.35</v>
       </c>
     </row>
@@ -1015,113 +1011,113 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Ingresa tu base gravable en la celda B4 y observa cómo las fórmulas calculan el ISR automáticamente.</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Base Gravable (ingreso acumulable - deducciones)</t>
         </is>
       </c>
-      <c r="B4" s="9" t="n">
+      <c r="B4" s="6" t="n">
         <v>450000</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>Límite Inferior (BUSCARV)</t>
         </is>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="7">
         <f>VLOOKUP(B4,Tarifa_Anual_2026,1,TRUE)</f>
         <v/>
       </c>
-      <c r="C5" s="7" t="inlineStr">
+      <c r="C5" s="4" t="inlineStr">
         <is>
           <t>BUSCARV busca el límite inferior que corresponde a tu ingreso</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>Excedente sobre Límite Inferior</t>
         </is>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="7">
         <f>B4-B5</f>
         <v/>
       </c>
-      <c r="C6" s="7" t="inlineStr">
+      <c r="C6" s="4" t="inlineStr">
         <is>
           <t>Tu ingreso menos el límite inferior de tu rango</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="inlineStr">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>% Sobre Excedente (BUSCARV)</t>
         </is>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="8">
         <f>VLOOKUP(B4,Tarifa_Anual_2026,4,TRUE)</f>
         <v/>
       </c>
-      <c r="C7" s="7" t="inlineStr">
+      <c r="C7" s="4" t="inlineStr">
         <is>
           <t>El porcentaje de impuesto sobre el excedente</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="inlineStr">
+      <c r="A8" s="5" t="inlineStr">
         <is>
           <t>ISR Marginal</t>
         </is>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <f>B6*B7</f>
         <v/>
       </c>
-      <c r="C8" s="7" t="inlineStr">
+      <c r="C8" s="4" t="inlineStr">
         <is>
           <t>Excedente × Porcentaje = ISR marginal</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="inlineStr">
+      <c r="A9" s="5" t="inlineStr">
         <is>
           <t>Cuota Fija (BUSCARV)</t>
         </is>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="7">
         <f>VLOOKUP(B4,Tarifa_Anual_2026,3,TRUE)</f>
         <v/>
       </c>
-      <c r="C9" s="7" t="inlineStr">
+      <c r="C9" s="4" t="inlineStr">
         <is>
           <t>Cantidad fija que se suma según tu rango</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="inlineStr">
+      <c r="A10" s="5" t="inlineStr">
         <is>
           <t>ISR del Ejercicio</t>
         </is>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="9">
         <f>B8+B9</f>
         <v/>
       </c>
-      <c r="C10" s="7" t="inlineStr">
+      <c r="C10" s="4" t="inlineStr">
         <is>
           <t>ISR Marginal + Cuota Fija = ISR Total del ejercicio</t>
         </is>
@@ -1162,85 +1158,85 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>El factor se trunca a 4 decimales (diezmilésimo) conforme al CFF.</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>INPC Reciente (Dic 2025)</t>
         </is>
       </c>
-      <c r="B4" s="13" t="n">
+      <c r="B4" s="10" t="n">
         <v>141.2</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>INPC Anterior (Dic 2024)</t>
         </is>
       </c>
-      <c r="B5" s="13" t="n">
+      <c r="B5" s="10" t="n">
         <v>136.163</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>Factor de Actualización (sin truncar)</t>
         </is>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <f>B4/B5</f>
         <v/>
       </c>
-      <c r="C6" s="7" t="inlineStr">
+      <c r="C6" s="4" t="inlineStr">
         <is>
           <t>División simple INPC reciente / INPC anterior</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="inlineStr">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>Factor de Actualización (TRUNCAR a 4 dec)</t>
         </is>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <f>TRUNC(B4/B5,4)</f>
         <v/>
       </c>
-      <c r="C7" s="7" t="inlineStr">
+      <c r="C7" s="4" t="inlineStr">
         <is>
           <t>TRUNCAR(valor, 4) — trunca sin redondear, como exige el CFF</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="inlineStr">
+      <c r="A9" s="5" t="inlineStr">
         <is>
           <t>Monto Original</t>
         </is>
       </c>
-      <c r="B9" s="16" t="n">
+      <c r="B9" s="13" t="n">
         <v>100000</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="inlineStr">
+      <c r="A10" s="5" t="inlineStr">
         <is>
           <t>Monto Actualizado</t>
         </is>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="14">
         <f>B9*B7</f>
         <v/>
       </c>
-      <c r="C10" s="7" t="inlineStr">
+      <c r="C10" s="4" t="inlineStr">
         <is>
           <t>Monto × Factor = Monto actualizado por inflación</t>
         </is>
@@ -1285,7 +1281,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Calcula el ISR para cada escenario. Usa BUSCARV con la tarifa anual.</t>
         </is>
@@ -1293,163 +1289,163 @@
     </row>
     <row r="3"/>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="15" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="15" t="inlineStr">
         <is>
           <t>Escenario</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="15" t="inlineStr">
         <is>
           <t>Ingreso Anual</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D4" s="15" t="inlineStr">
         <is>
           <t>Deducciones</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="E4" s="15" t="inlineStr">
         <is>
           <t>Base Gravable</t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" s="15" t="inlineStr">
         <is>
           <t>ISR (tu respuesta)</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
+      <c r="G4" s="15" t="inlineStr">
         <is>
           <t>ISR (verificación)</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="18" t="n">
+      <c r="A5" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="18" t="inlineStr">
+      <c r="B5" s="16" t="inlineStr">
         <is>
           <t>Empleado con sueldo fijo</t>
         </is>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="17" t="n">
         <v>280000</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="17" t="n">
         <v>45000</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="17">
         <f>C5-D5</f>
         <v/>
       </c>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="3">
+      <c r="F5" s="17" t="n"/>
+      <c r="G5" s="17">
         <f>VLOOKUP(E5,Tarifa_Anual_2026,3,TRUE)+(E5-VLOOKUP(E5,Tarifa_Anual_2026,1,TRUE))*VLOOKUP(E5,Tarifa_Anual_2026,4,TRUE)</f>
         <v/>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="19" t="n">
+      <c r="A6" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="19" t="inlineStr">
+      <c r="B6" s="18" t="inlineStr">
         <is>
           <t>Freelancer con ingresos variables</t>
         </is>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="19" t="n">
         <v>520000</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="19" t="n">
         <v>120000</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="19">
         <f>C6-D6</f>
         <v/>
       </c>
-      <c r="F6" s="5" t="n"/>
-      <c r="G6" s="5">
+      <c r="F6" s="19" t="n"/>
+      <c r="G6" s="19">
         <f>VLOOKUP(E6,Tarifa_Anual_2026,3,TRUE)+(E6-VLOOKUP(E6,Tarifa_Anual_2026,1,TRUE))*VLOOKUP(E6,Tarifa_Anual_2026,4,TRUE)</f>
         <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="18" t="n">
+      <c r="A7" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="18" t="inlineStr">
+      <c r="B7" s="16" t="inlineStr">
         <is>
           <t>Socio de empresa (dividendos)</t>
         </is>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="17" t="n">
         <v>1500000</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="17" t="n">
         <v>350000</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="17">
         <f>C7-D7</f>
         <v/>
       </c>
-      <c r="F7" s="3" t="n"/>
-      <c r="G7" s="3">
+      <c r="F7" s="17" t="n"/>
+      <c r="G7" s="17">
         <f>VLOOKUP(E7,Tarifa_Anual_2026,3,TRUE)+(E7-VLOOKUP(E7,Tarifa_Anual_2026,1,TRUE))*VLOOKUP(E7,Tarifa_Anual_2026,4,TRUE)</f>
         <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="19" t="n">
+      <c r="A8" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="19" t="inlineStr">
+      <c r="B8" s="18" t="inlineStr">
         <is>
           <t>Trabajador zona fronteriza</t>
         </is>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="19" t="n">
         <v>180000</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="19" t="n">
         <v>30000</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="19">
         <f>C8-D8</f>
         <v/>
       </c>
-      <c r="F8" s="5" t="n"/>
-      <c r="G8" s="5">
+      <c r="F8" s="19" t="n"/>
+      <c r="G8" s="19">
         <f>VLOOKUP(E8,Tarifa_Anual_2026,3,TRUE)+(E8-VLOOKUP(E8,Tarifa_Anual_2026,1,TRUE))*VLOOKUP(E8,Tarifa_Anual_2026,4,TRUE)</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="18" t="n">
+      <c r="A9" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="18" t="inlineStr">
+      <c r="B9" s="16" t="inlineStr">
         <is>
           <t>Director general (ingreso alto)</t>
         </is>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="17" t="n">
         <v>3200000</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="17" t="n">
         <v>600000</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="17">
         <f>C9-D9</f>
         <v/>
       </c>
-      <c r="F9" s="3" t="n"/>
-      <c r="G9" s="3">
+      <c r="F9" s="17" t="n"/>
+      <c r="G9" s="17">
         <f>VLOOKUP(E9,Tarifa_Anual_2026,3,TRUE)+(E9-VLOOKUP(E9,Tarifa_Anual_2026,1,TRUE))*VLOOKUP(E9,Tarifa_Anual_2026,4,TRUE)</f>
         <v/>
       </c>

</xml_diff>